<commit_message>
PDF of HighF filter/gain/hydrophone character
</commit_message>
<xml_diff>
--- a/HighFCalcs.xlsx
+++ b/HighFCalcs.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="4.3" sheetId="1" r:id="rId1"/>
+    <sheet name="4.4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>f(kHz)</t>
   </si>
@@ -45,6 +46,9 @@
   </si>
   <si>
     <t>R2</t>
+  </si>
+  <si>
+    <t>R2(kOhm)</t>
   </si>
 </sst>
 </file>
@@ -74,7 +78,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -82,15 +86,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,7 +245,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$28</c:f>
+              <c:f>'4.3'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
@@ -303,7 +335,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$28</c:f>
+              <c:f>'4.3'!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
@@ -574,7 +606,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -645,8 +677,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1807012248468941"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.18903455818022746"/>
+          <c:y val="4.6296296296296294E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -713,7 +745,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$32:$A$58</c:f>
+              <c:f>'4.3'!$A$32:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
@@ -803,7 +835,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$32:$B$58</c:f>
+              <c:f>'4.3'!$B$32:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
@@ -1079,6 +1111,1584 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>High F Gain Rx</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'4.4'!$A$2:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'4.4'!$B$2:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>57.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-499F-48D2-92DF-BCA270557965}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="393077088"/>
+        <c:axId val="393079712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="393077088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="393079712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="393079712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="393077088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>High F</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Gain Rx - F</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'4.4'!$K$2:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'4.4'!$L$2:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>57.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-57C3-4DDF-8C9F-F8442AAE2966}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="342260280"/>
+        <c:axId val="342261920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="342260280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="342261920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="342261920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="342260280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Overlay</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.43798214727786733"/>
+          <c:y val="2.5157232704402517E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'4.4'!$K$2:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'4.4'!$L$2:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>57.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D1C-46C9-A473-A49CAC36ED13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>NoFix</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'4.4'!$A$2:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'4.4'!$B$2:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>57.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2D1C-46C9-A473-A49CAC36ED13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="397979472"/>
+        <c:axId val="397974880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="397979472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397974880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="397974880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397979472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1159,6 +2769,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1676,6 +3406,1554 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2196,15 +5474,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2226,15 +5504,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>338137</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>385762</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2248,6 +5526,101 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>100011</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2521,8 +5894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2586,6 +5959,19 @@
       <c r="B4">
         <v>62</v>
       </c>
+      <c r="L4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1.4400000000000001E-3</v>
+      </c>
+      <c r="N4" s="1">
+        <v>8.7100000000000007E-3</v>
+      </c>
+      <c r="O4" s="1">
+        <f>((N4/M4)-1)*L4</f>
+        <v>5048.6111111111113</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2594,6 +5980,19 @@
       <c r="B5">
         <v>62</v>
       </c>
+      <c r="L5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="N5" s="1">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="O5" s="1">
+        <f>((N5/M5)-1)*L5</f>
+        <v>4866.666666666667</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2602,6 +6001,19 @@
       <c r="B6">
         <v>106</v>
       </c>
+      <c r="L6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5.1200000000000004E-3</v>
+      </c>
+      <c r="N6" s="1">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="O6" s="1">
+        <f>((N6/M6)-1)*L6</f>
+        <v>5132.8124999999991</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2998,6 +6410,375 @@
       </c>
       <c r="B58">
         <v>19.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>57.6</v>
+      </c>
+      <c r="C2">
+        <v>5.13</v>
+      </c>
+      <c r="K2">
+        <v>30</v>
+      </c>
+      <c r="L2">
+        <v>57.6</v>
+      </c>
+      <c r="M2">
+        <v>5.13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>21.6</v>
+      </c>
+      <c r="K3" s="4">
+        <v>31</v>
+      </c>
+      <c r="L3" s="5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>64</v>
+      </c>
+      <c r="K4">
+        <v>32</v>
+      </c>
+      <c r="L4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>89.6</v>
+      </c>
+      <c r="K5">
+        <v>33</v>
+      </c>
+      <c r="L5">
+        <v>89.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>50.4</v>
+      </c>
+      <c r="K6">
+        <v>34</v>
+      </c>
+      <c r="L6">
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>96.5</v>
+      </c>
+      <c r="K7">
+        <v>35</v>
+      </c>
+      <c r="L7">
+        <v>96.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>98</v>
+      </c>
+      <c r="K8">
+        <v>36</v>
+      </c>
+      <c r="L8">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>186</v>
+      </c>
+      <c r="K9">
+        <v>37</v>
+      </c>
+      <c r="L9">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>70</v>
+      </c>
+      <c r="K10" s="4">
+        <v>38</v>
+      </c>
+      <c r="L10" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>128</v>
+      </c>
+      <c r="K11">
+        <v>39</v>
+      </c>
+      <c r="L11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>120</v>
+      </c>
+      <c r="K12" s="3">
+        <v>40</v>
+      </c>
+      <c r="L12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>232</v>
+      </c>
+      <c r="K13" s="3">
+        <v>41</v>
+      </c>
+      <c r="L13">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>154</v>
+      </c>
+      <c r="K14" s="3">
+        <v>42</v>
+      </c>
+      <c r="L14">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>43</v>
+      </c>
+      <c r="B15">
+        <v>196</v>
+      </c>
+      <c r="K15" s="3">
+        <v>43</v>
+      </c>
+      <c r="L15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>126</v>
+      </c>
+      <c r="K16">
+        <v>44</v>
+      </c>
+      <c r="L16">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>350</v>
+      </c>
+      <c r="K17">
+        <v>45</v>
+      </c>
+      <c r="L17">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>46</v>
+      </c>
+      <c r="B18">
+        <v>24</v>
+      </c>
+      <c r="K18" s="4">
+        <v>46</v>
+      </c>
+      <c r="L18" s="5">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>82</v>
+      </c>
+      <c r="K19">
+        <v>47</v>
+      </c>
+      <c r="L19">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>82</v>
+      </c>
+      <c r="K20">
+        <v>48</v>
+      </c>
+      <c r="L20">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>49</v>
+      </c>
+      <c r="B21">
+        <v>106</v>
+      </c>
+      <c r="K21">
+        <v>49</v>
+      </c>
+      <c r="L21">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>50</v>
+      </c>
+      <c r="B22">
+        <v>140</v>
+      </c>
+      <c r="K22">
+        <v>50</v>
+      </c>
+      <c r="L22">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>132</v>
+      </c>
+      <c r="K23">
+        <v>51</v>
+      </c>
+      <c r="L23">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>52</v>
+      </c>
+      <c r="B24">
+        <v>76</v>
+      </c>
+      <c r="K24">
+        <v>52</v>
+      </c>
+      <c r="L24">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FSKRx2, Gain PDF, graphs edited
</commit_message>
<xml_diff>
--- a/HighFCalcs.xlsx
+++ b/HighFCalcs.xlsx
@@ -9,13 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="4.3" sheetId="1" r:id="rId1"/>
     <sheet name="4.4" sheetId="2" r:id="rId2"/>
+    <sheet name="4.5" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="4.7" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>f(kHz)</t>
   </si>
@@ -49,6 +53,21 @@
   </si>
   <si>
     <t>R2(kOhm)</t>
+  </si>
+  <si>
+    <t>gain</t>
+  </si>
+  <si>
+    <t>vin</t>
+  </si>
+  <si>
+    <t>vout</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -180,7 +199,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1151,7 +1169,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1373,7 +1390,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-499F-48D2-92DF-BCA270557965}"/>
+              <c16:uniqueId val="{00000000-8179-40BD-B055-0C51DD1D9822}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1593,6 +1610,452 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>High F Gain Rx</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'4.4'!$A$2:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'4.4'!$B$2:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>57.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-499F-48D2-92DF-BCA270557965}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="393077088"/>
+        <c:axId val="393079712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="393077088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="393079712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="393079712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="393077088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>High F</a:t>
             </a:r>
             <a:r>
@@ -1603,7 +2066,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2010,7 +2472,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2622,7 +3084,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2652,6 +3113,471 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vout (mV) v.  Fin (kHz) - Gain 10x</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'4.5'!$A$2:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'4.5'!$B$2:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8324-48A8-9A2A-F8C1C9FE8738}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="377896088"/>
+        <c:axId val="377892480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="377896088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377892480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="377892480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377896088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2889,6 +3815,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4954,6 +5960,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5526,6 +7564,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5621,6 +7691,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5892,15 +7997,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5911,7 +8016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>30</v>
       </c>
@@ -5931,7 +8036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>31</v>
       </c>
@@ -5952,7 +8057,7 @@
         <v>4760.6382978723404</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>32</v>
       </c>
@@ -5973,7 +8078,7 @@
         <v>5048.6111111111113</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>33</v>
       </c>
@@ -5994,7 +8099,7 @@
         <v>4866.666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>34</v>
       </c>
@@ -6015,23 +8120,47 @@
         <v>5132.8124999999991</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>35</v>
       </c>
       <c r="B7">
         <v>148</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1.3650000000000001E-2</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="O7" s="1">
+        <f>((N7/M7)-1)*L7</f>
+        <v>9183.1501831501846</v>
+      </c>
+      <c r="Q7" s="1">
+        <f>N7/(0.004)</f>
+        <v>34.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>36</v>
       </c>
       <c r="B8">
         <v>106</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q8" s="1">
+        <v>1.2329999999999999E-3</v>
+      </c>
+      <c r="R8" s="1">
+        <f>Q8*34.8</f>
+        <v>4.2908399999999992E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>37</v>
       </c>
@@ -6039,7 +8168,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>38</v>
       </c>
@@ -6047,7 +8176,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>39</v>
       </c>
@@ -6055,7 +8184,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>40</v>
       </c>
@@ -6063,7 +8192,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>41</v>
       </c>
@@ -6071,7 +8200,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42</v>
       </c>
@@ -6079,7 +8208,7 @@
         <v>94.4</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43</v>
       </c>
@@ -6087,7 +8216,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>44</v>
       </c>
@@ -6423,8 +8552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6785,4 +8914,536 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>43</v>
+      </c>
+      <c r="B15">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>46</v>
+      </c>
+      <c r="B18">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>49</v>
+      </c>
+      <c r="B21">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>50</v>
+      </c>
+      <c r="B22">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>52</v>
+      </c>
+      <c r="B24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>54</v>
+      </c>
+      <c r="B25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>55</v>
+      </c>
+      <c r="B26">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>56</v>
+      </c>
+      <c r="B27">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="B2">
+        <v>0.53</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2/A2</f>
+        <v>94.642857142857153</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3.2700000000000002E-5</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F7" si="0">1/E2</f>
+        <v>30581.039755351681</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <f>B3/A3</f>
+        <v>3.1213872832369942</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="0"/>
+        <v>99999.999999999985</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.4E-3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <f>B4/A4</f>
+        <v>15.714285714285714</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.0200000000000001E-5</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>98039.215686274503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="B5">
+        <v>12.7</v>
+      </c>
+      <c r="C5" s="1">
+        <f>B5/A5</f>
+        <v>15.301204819277109</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6.1199999999999997E-5</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>16339.869281045752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>5.6400000000000002E-5</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>17730.496453900709</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>1.8E-5</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>55555.555555555555</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1.6800000000000001E-3</v>
+      </c>
+      <c r="B1" s="1">
+        <f t="shared" ref="B1:B17" si="0">1/A1</f>
+        <v>595.23809523809518</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>8.6000000000000007E-6</v>
+      </c>
+      <c r="B2" s="1">
+        <f t="shared" si="0"/>
+        <v>116279.06976744185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1.1E-5</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" si="0"/>
+        <v>90909.090909090912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>27777.777777777777</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3.44E-2</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>29.069767441860463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5.5999999999999995E-4</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>1785.7142857142858</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2.0800000000000001E-5</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>48076.923076923078</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1.3799999999999999E-4</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>7246.376811594203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2.16E-5</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>46296.296296296299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>49999.999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>45454.545454545456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.66E-2</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>60.240963855421683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>4.4000000000000002E-4</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>2272.7272727272725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>1111.1111111111111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2.26E-5</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>44247.787610619467</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>9.6399999999999992E-6</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>103734.4398340249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>